<commit_message>
fixing an issue that showed spending and revenue twice and adding in a bit more granular details to the spend
</commit_message>
<xml_diff>
--- a/data/montreal/data_cleaning/montreal_financial_statement_data_2024.xlsx
+++ b/data/montreal/data_cleaning/montreal_financial_statement_data_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boris\Projects\CanadaSpends\data\montreal\data_cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4640353B-AA58-4ADB-8E47-36B1CB87AD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839227DD-0962-40E4-A6C3-FC0EA27AC895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{BF1821EE-C325-4E8C-A214-4DEB8EEAC78D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BF1821EE-C325-4E8C-A214-4DEB8EEAC78D}"/>
   </bookViews>
   <sheets>
     <sheet name="Checker" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Expenses" sheetId="3" r:id="rId5"/>
     <sheet name="tca_net_calculation" sheetId="5" r:id="rId6"/>
     <sheet name="2024_financial_report_raw_data" sheetId="1" r:id="rId7"/>
-    <sheet name="miscellaneous" sheetId="4" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="miscellaneous" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">tca_net_calculation!$B$4:$F$17</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="183">
   <si>
     <t>Revenue</t>
   </si>
@@ -589,6 +590,12 @@
   </si>
   <si>
     <t>sankey_5</t>
+  </si>
+  <si>
+    <t>Municipal administration less Eliminations</t>
+  </si>
+  <si>
+    <t>Urban planning and Development</t>
   </si>
 </sst>
 </file>
@@ -657,14 +664,12 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1033,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <f>SUMIFS(cleaned_data!$F$2:$F$51,cleaned_data!$E$2:$E$51,Checker!B4)</f>
+        <f>SUMIFS(cleaned_data!$F$2:$F$56,cleaned_data!$E$2:$E$56,Checker!B4)</f>
         <v>9803882</v>
       </c>
     </row>
@@ -1042,7 +1047,7 @@
         <v>164</v>
       </c>
       <c r="C5" s="2">
-        <f>SUMIFS(cleaned_data!$F$2:$F$51,cleaned_data!$E$2:$E$51,Checker!B5)</f>
+        <f>SUMIFS(cleaned_data!$F$2:$F$56,cleaned_data!$E$2:$E$56,Checker!B5)</f>
         <v>10691929</v>
       </c>
     </row>
@@ -1082,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8845F93-8333-4F82-B301-EF277042A533}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1358,7 @@
       <c r="A16" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>80</v>
       </c>
       <c r="C16" t="s">
@@ -1376,7 +1381,7 @@
       <c r="A17" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>80</v>
       </c>
       <c r="C17" t="s">
@@ -1399,7 +1404,7 @@
       <c r="A18" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>80</v>
       </c>
       <c r="C18" t="s">
@@ -1422,7 +1427,7 @@
       <c r="A19" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>80</v>
       </c>
       <c r="C19" t="s">
@@ -1445,7 +1450,7 @@
       <c r="A20" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>80</v>
       </c>
       <c r="C20" t="s">
@@ -1468,7 +1473,7 @@
       <c r="A21" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>75</v>
       </c>
       <c r="C21" t="s">
@@ -1491,7 +1496,7 @@
       <c r="A22" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
       <c r="C22" t="s">
@@ -1512,7 +1517,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="5" t="s">
+      <c r="C23" t="s">
         <v>92</v>
       </c>
       <c r="D23" t="s">
@@ -1529,7 +1534,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="5" t="s">
+      <c r="C24" t="s">
         <v>93</v>
       </c>
       <c r="D24" t="s">
@@ -1546,7 +1551,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
+      <c r="C25" t="s">
         <v>95</v>
       </c>
       <c r="D25" t="s">
@@ -1563,7 +1568,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="5" t="s">
+      <c r="C26" t="s">
         <v>96</v>
       </c>
       <c r="D26" t="s">
@@ -1617,7 +1622,7 @@
       <c r="D29" t="s">
         <v>149</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" t="s">
         <v>154</v>
       </c>
       <c r="F29" s="2">
@@ -1637,7 +1642,7 @@
       <c r="D30" t="s">
         <v>149</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" t="s">
         <v>154</v>
       </c>
       <c r="F30" s="2">
@@ -1648,6 +1653,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>181</v>
+      </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
@@ -1662,6 +1670,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>181</v>
+      </c>
       <c r="C32" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +1686,10 @@
         <v>1364228</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>181</v>
+      </c>
       <c r="C33" t="s">
         <v>14</v>
       </c>
@@ -1686,12 +1700,15 @@
         <v>148</v>
       </c>
       <c r="F33" s="2">
-        <v>3612593</v>
-      </c>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+        <v>1527772</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
         <v>151</v>
@@ -1700,12 +1717,15 @@
         <v>148</v>
       </c>
       <c r="F34" s="2">
-        <v>684792</v>
-      </c>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+        <v>2084821</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>181</v>
+      </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
         <v>151</v>
@@ -1714,12 +1734,15 @@
         <v>148</v>
       </c>
       <c r="F35" s="2">
-        <v>333470</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+        <v>684792</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>181</v>
+      </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
         <v>151</v>
@@ -1728,12 +1751,15 @@
         <v>148</v>
       </c>
       <c r="F36" s="2">
-        <v>330257</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+        <v>255728</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
         <v>151</v>
@@ -1742,12 +1768,15 @@
         <v>148</v>
       </c>
       <c r="F37" s="2">
-        <v>1006407</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+        <v>77742</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>181</v>
+      </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>182</v>
       </c>
       <c r="D38" t="s">
         <v>151</v>
@@ -1756,162 +1785,162 @@
         <v>148</v>
       </c>
       <c r="F38" s="2">
-        <v>572070</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+        <v>326899</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="D39" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E39" t="s">
         <v>148</v>
       </c>
       <c r="F39" s="2">
-        <v>38132</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>181</v>
+      </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E40" t="s">
         <v>148</v>
       </c>
       <c r="F40" s="2">
-        <v>13648</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+        <v>922615</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E41" t="s">
         <v>148</v>
       </c>
       <c r="F41" s="2">
-        <v>138936</v>
-      </c>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+        <v>83792</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>181</v>
+      </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E42" t="s">
         <v>148</v>
       </c>
       <c r="F42" s="2">
-        <v>4140</v>
-      </c>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+        <v>375578</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
       <c r="C43" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>149</v>
+        <v>18</v>
+      </c>
+      <c r="D43" t="s">
+        <v>151</v>
       </c>
       <c r="E43" t="s">
         <v>148</v>
       </c>
       <c r="F43" s="2">
-        <v>831751</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+        <v>196492</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>66</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>149</v>
+        <v>26</v>
+      </c>
+      <c r="D44" t="s">
+        <v>150</v>
       </c>
       <c r="E44" t="s">
         <v>148</v>
       </c>
       <c r="F44" s="2">
-        <v>437653</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+        <v>38132</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="D45" t="s">
+        <v>150</v>
       </c>
       <c r="E45" t="s">
         <v>148</v>
       </c>
       <c r="F45" s="2">
-        <v>4418</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+        <v>13648</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>149</v>
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>150</v>
       </c>
       <c r="E46" t="s">
         <v>148</v>
       </c>
       <c r="F46" s="2">
-        <v>340173</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+        <v>138936</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>70</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>149</v>
+        <v>29</v>
+      </c>
+      <c r="D47" t="s">
+        <v>150</v>
       </c>
       <c r="E47" t="s">
         <v>148</v>
       </c>
       <c r="F47" s="2">
-        <v>18865</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" t="s">
         <v>149</v>
       </c>
       <c r="E48" t="s">
         <v>148</v>
       </c>
       <c r="F48" s="2">
-        <v>15910</v>
+        <v>831751</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>159</v>
@@ -1919,16 +1948,16 @@
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" t="s">
         <v>149</v>
       </c>
       <c r="E49" t="s">
         <v>148</v>
       </c>
       <c r="F49" s="2">
-        <v>11488</v>
+        <v>437653</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>159</v>
@@ -1936,16 +1965,16 @@
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>74</v>
-      </c>
-      <c r="D50" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" t="s">
         <v>149</v>
       </c>
       <c r="E50" t="s">
         <v>148</v>
       </c>
       <c r="F50" s="2">
-        <v>113205</v>
+        <v>4418</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>159</v>
@@ -1953,18 +1982,103 @@
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" t="s">
         <v>149</v>
       </c>
       <c r="E51" t="s">
         <v>148</v>
       </c>
       <c r="F51" s="2">
+        <v>340173</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" t="s">
+        <v>148</v>
+      </c>
+      <c r="F52" s="2">
+        <v>18865</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" t="s">
+        <v>148</v>
+      </c>
+      <c r="F53" s="2">
+        <v>15910</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" t="s">
+        <v>148</v>
+      </c>
+      <c r="F54" s="2">
+        <v>11488</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" t="s">
+        <v>148</v>
+      </c>
+      <c r="F55" s="2">
+        <v>113205</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" t="s">
+        <v>148</v>
+      </c>
+      <c r="F56" s="2">
         <v>9385</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1992,7 +2106,7 @@
         <v>164</v>
       </c>
       <c r="C2" s="2">
-        <f>SUMIFS(cleaned_data!$F$2:$F$51,cleaned_data!$E$2:$E$51,tables_for_summary!B2)</f>
+        <f>SUMIFS(cleaned_data!$F$2:$F$56,cleaned_data!$E$2:$E$56,tables_for_summary!B2)</f>
         <v>10691929</v>
       </c>
     </row>
@@ -2001,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <f>SUMIFS(cleaned_data!$F$2:$F$51,cleaned_data!$E$2:$E$51,tables_for_summary!B3)</f>
+        <f>SUMIFS(cleaned_data!$F$2:$F$56,cleaned_data!$E$2:$E$56,tables_for_summary!B3)</f>
         <v>9803882</v>
       </c>
     </row>
@@ -2058,7 +2172,7 @@
       <c r="D9" t="s">
         <v>175</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2069,7 +2183,7 @@
       <c r="C11" s="2">
         <v>810408</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <f>C11/$C$2</f>
         <v>7.5796238452387782E-2</v>
       </c>
@@ -2081,7 +2195,7 @@
       <c r="C12" s="2">
         <v>1364228</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <f t="shared" ref="D12:D17" si="0">C12/$C$2</f>
         <v>0.12759418810207213</v>
       </c>
@@ -2093,7 +2207,7 @@
       <c r="C13" s="2">
         <v>3612593</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="7">
         <f t="shared" si="0"/>
         <v>0.33788037687118949</v>
       </c>
@@ -2105,7 +2219,7 @@
       <c r="C14" s="2">
         <v>684792</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="7">
         <f t="shared" si="0"/>
         <v>6.4047563353628698E-2</v>
       </c>
@@ -2117,7 +2231,7 @@
       <c r="C15" s="2">
         <v>333470</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <f t="shared" si="0"/>
         <v>3.1188946353833812E-2</v>
       </c>
@@ -2129,7 +2243,7 @@
       <c r="C16" s="2">
         <v>330257</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="7">
         <f t="shared" si="0"/>
         <v>3.0888439307818073E-2</v>
       </c>
@@ -2141,7 +2255,7 @@
       <c r="C17" s="2">
         <v>1006407</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <f t="shared" si="0"/>
         <v>9.4127729430302051E-2</v>
       </c>
@@ -2160,7 +2274,7 @@
   <dimension ref="A2:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,7 +2546,7 @@
       <c r="A18" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>80</v>
       </c>
       <c r="C18" t="s">
@@ -2455,7 +2569,7 @@
       <c r="A19" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>80</v>
       </c>
       <c r="C19" t="s">
@@ -2478,7 +2592,7 @@
       <c r="A20" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>80</v>
       </c>
       <c r="C20" t="s">
@@ -2501,7 +2615,7 @@
       <c r="A21" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>80</v>
       </c>
       <c r="C21" t="s">
@@ -2524,7 +2638,7 @@
       <c r="A22" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>80</v>
       </c>
       <c r="C22" t="s">
@@ -2547,7 +2661,7 @@
       <c r="A23" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>75</v>
       </c>
       <c r="C23" t="s">
@@ -2570,7 +2684,7 @@
       <c r="A24" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>75</v>
       </c>
       <c r="C24" t="s">
@@ -2591,7 +2705,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
+      <c r="C25" t="s">
         <v>92</v>
       </c>
       <c r="D25" t="s">
@@ -2608,7 +2722,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="5" t="s">
+      <c r="C26" t="s">
         <v>93</v>
       </c>
       <c r="D26" t="s">
@@ -2625,7 +2739,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="5" t="s">
+      <c r="C27" t="s">
         <v>95</v>
       </c>
       <c r="D27" t="s">
@@ -2642,7 +2756,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="5" t="s">
+      <c r="C28" t="s">
         <v>96</v>
       </c>
       <c r="D28" t="s">
@@ -2696,7 +2810,7 @@
       <c r="D31" t="s">
         <v>149</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" t="s">
         <v>154</v>
       </c>
       <c r="F31" s="2">
@@ -2716,7 +2830,7 @@
       <c r="D32" t="s">
         <v>149</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" t="s">
         <v>154</v>
       </c>
       <c r="F32" s="2">
@@ -2741,10 +2855,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD175C9-8012-4A98-B7F2-438C43D6DA3B}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,7 +2870,7 @@
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>180</v>
       </c>
@@ -2780,7 +2894,10 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
@@ -2794,7 +2911,10 @@
         <v>810408</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
@@ -2808,7 +2928,10 @@
         <v>1364228</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
@@ -2819,12 +2942,15 @@
         <v>148</v>
       </c>
       <c r="F4" s="2">
-        <v>3612593</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1527772</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>151</v>
@@ -2833,12 +2959,15 @@
         <v>148</v>
       </c>
       <c r="F5" s="2">
-        <v>684792</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2084821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>181</v>
+      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>151</v>
@@ -2847,12 +2976,15 @@
         <v>148</v>
       </c>
       <c r="F6" s="2">
-        <v>333470</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>684792</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>151</v>
@@ -2861,12 +2993,15 @@
         <v>148</v>
       </c>
       <c r="F7" s="2">
-        <v>330257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>255728</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>151</v>
@@ -2875,12 +3010,15 @@
         <v>148</v>
       </c>
       <c r="F8" s="2">
-        <v>1006407</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>77742</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>181</v>
+      </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>182</v>
       </c>
       <c r="D9" t="s">
         <v>151</v>
@@ -2889,249 +3027,313 @@
         <v>148</v>
       </c>
       <c r="F9" s="2">
-        <v>572070</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>326899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E10" t="s">
         <v>148</v>
       </c>
       <c r="F10" s="2">
-        <v>38132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E11" t="s">
         <v>148</v>
       </c>
       <c r="F11" s="2">
-        <v>13648</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>922615</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E12" t="s">
         <v>148</v>
       </c>
       <c r="F12" s="2">
-        <v>138936</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83792</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E13" t="s">
         <v>148</v>
       </c>
       <c r="F13" s="2">
-        <v>4140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>375578</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
       <c r="C14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>149</v>
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>151</v>
       </c>
       <c r="E14" t="s">
         <v>148</v>
       </c>
       <c r="F14" s="2">
-        <v>831751</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>196492</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>149</v>
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>150</v>
       </c>
       <c r="E15" t="s">
         <v>148</v>
       </c>
       <c r="F15" s="2">
-        <v>437653</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>149</v>
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>150</v>
       </c>
       <c r="E16" t="s">
         <v>148</v>
       </c>
       <c r="F16" s="2">
-        <v>4418</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+        <v>13648</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>149</v>
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>150</v>
       </c>
       <c r="E17" t="s">
         <v>148</v>
       </c>
       <c r="F17" s="2">
-        <v>340173</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+        <v>138936</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>149</v>
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
       </c>
       <c r="E18" t="s">
         <v>148</v>
       </c>
       <c r="F18" s="2">
-        <v>18865</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
         <v>149</v>
       </c>
       <c r="E19" t="s">
         <v>148</v>
       </c>
       <c r="F19" s="2">
-        <v>15910</v>
+        <v>831751</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
         <v>149</v>
       </c>
       <c r="E20" t="s">
         <v>148</v>
       </c>
       <c r="F20" s="2">
-        <v>11488</v>
+        <v>437653</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
         <v>149</v>
       </c>
       <c r="E21" t="s">
         <v>148</v>
       </c>
       <c r="F21" s="2">
-        <v>113205</v>
+        <v>4418</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
         <v>149</v>
       </c>
       <c r="E22" t="s">
         <v>148</v>
       </c>
       <c r="F22" s="2">
-        <v>9385</v>
+        <v>340173</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="2">
+        <v>18865</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="2">
+        <v>15910</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F25" s="2">
+        <v>11488</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="2">
+        <v>113205</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>149</v>
+      </c>
+      <c r="E27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="2">
+        <v>9385</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
@@ -3149,7 +3351,13 @@
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="4"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="2"/>
     </row>
     <row r="41" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>
@@ -3159,30 +3367,6 @@
     </row>
     <row r="43" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F51" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3193,7 +3377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA991F28-B0AD-4115-91E6-AD205E4FCAA1}">
   <dimension ref="B4:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -3526,8 +3710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D1A74A-9D2A-4B83-9414-C5BA674674D0}">
   <dimension ref="A1:E273"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:B29"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3932,10 +4116,10 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="A45" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="2">
         <v>172151</v>
       </c>
     </row>
@@ -3965,7 +4149,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" t="s">
         <v>38</v>
       </c>
       <c r="B49" s="2">
@@ -4032,7 +4216,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="A57" t="s">
         <v>38</v>
       </c>
       <c r="B57" s="2">
@@ -4065,7 +4249,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="A61" t="s">
         <v>38</v>
       </c>
       <c r="B61" s="2">
@@ -4098,7 +4282,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+      <c r="A65" t="s">
         <v>38</v>
       </c>
       <c r="B65" s="2">
@@ -4129,7 +4313,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="A69" t="s">
         <v>38</v>
       </c>
       <c r="B69" s="2">
@@ -4179,10 +4363,10 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+      <c r="A75" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="2">
         <v>11155</v>
       </c>
     </row>
@@ -4196,16 +4380,16 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="6">
         <f>B39+B41+B43+B47+B51+B53+B55+B59+B63+B66+B71+B73+B76</f>
         <v>9675870</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+      <c r="A78" t="s">
         <v>49</v>
       </c>
       <c r="B78" s="2">
@@ -4277,7 +4461,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+      <c r="A87" t="s">
         <v>38</v>
       </c>
       <c r="B87" s="2">
@@ -4335,7 +4519,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+      <c r="A94" t="s">
         <v>38</v>
       </c>
       <c r="B94" s="2">
@@ -4368,7 +4552,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
+      <c r="A98" t="s">
         <v>38</v>
       </c>
       <c r="B98" s="2">
@@ -4401,7 +4585,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
+      <c r="A102" t="s">
         <v>38</v>
       </c>
       <c r="B102" s="2">
@@ -4434,7 +4618,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+      <c r="A106" t="s">
         <v>38</v>
       </c>
       <c r="B106" s="2">
@@ -4459,19 +4643,19 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="7" t="s">
+      <c r="A109" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B109" s="8">
+      <c r="B109" s="6">
         <f>B82+B85+B89+B92+B96+B100+B104+B108</f>
         <v>8714225</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+      <c r="A110" t="s">
         <v>49</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="2">
         <f>B21</f>
         <v>8714225</v>
       </c>
@@ -4497,7 +4681,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
+      <c r="A115" t="s">
         <v>38</v>
       </c>
       <c r="B115" s="2">
@@ -4525,7 +4709,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
+      <c r="A118" t="s">
         <v>38</v>
       </c>
       <c r="B118" s="2">
@@ -4561,7 +4745,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
+      <c r="A122" t="s">
         <v>38</v>
       </c>
       <c r="B122" s="2">
@@ -4586,7 +4770,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
+      <c r="A125" t="s">
         <v>38</v>
       </c>
       <c r="B125" s="2">
@@ -4611,7 +4795,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
+      <c r="A128" t="s">
         <v>38</v>
       </c>
       <c r="B128" s="2">
@@ -4636,7 +4820,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
+      <c r="A131" t="s">
         <v>38</v>
       </c>
       <c r="B131" s="2">
@@ -4672,7 +4856,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
+      <c r="A135" t="s">
         <v>38</v>
       </c>
       <c r="B135" s="2">
@@ -4708,7 +4892,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="5" t="s">
+      <c r="A139" t="s">
         <v>38</v>
       </c>
       <c r="B139" s="2">
@@ -4744,7 +4928,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
+      <c r="A143" t="s">
         <v>38</v>
       </c>
       <c r="B143" s="2">
@@ -4780,7 +4964,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
+      <c r="A147" t="s">
         <v>38</v>
       </c>
       <c r="B147" s="2">
@@ -4836,7 +5020,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="5" t="s">
+      <c r="A153" t="s">
         <v>38</v>
       </c>
       <c r="B153" s="2">
@@ -4864,7 +5048,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
+      <c r="A156" t="s">
         <v>38</v>
       </c>
       <c r="B156" s="2">
@@ -4900,7 +5084,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
+      <c r="A160" t="s">
         <v>38</v>
       </c>
       <c r="B160" s="2">
@@ -4936,7 +5120,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
+      <c r="A164" t="s">
         <v>38</v>
       </c>
       <c r="B164" s="2">
@@ -4972,7 +5156,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="5" t="s">
+      <c r="A168" t="s">
         <v>38</v>
       </c>
       <c r="B168" s="2">
@@ -4995,7 +5179,7 @@
       <c r="A170" t="s">
         <v>33</v>
       </c>
-      <c r="B170" s="6">
+      <c r="B170" s="2">
         <v>76545</v>
       </c>
     </row>
@@ -5003,7 +5187,7 @@
       <c r="A171" t="s">
         <v>34</v>
       </c>
-      <c r="B171" s="6">
+      <c r="B171" s="2">
         <v>-53792</v>
       </c>
     </row>
@@ -5023,15 +5207,15 @@
       <c r="A173" t="s">
         <v>33</v>
       </c>
-      <c r="B173" s="6">
+      <c r="B173" s="2">
         <v>6307</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="5" t="s">
+      <c r="A174" t="s">
         <v>38</v>
       </c>
-      <c r="B174" s="6">
+      <c r="B174" s="2">
         <v>47685</v>
       </c>
     </row>
@@ -5048,7 +5232,7 @@
       <c r="A176" t="s">
         <v>33</v>
       </c>
-      <c r="B176" s="6">
+      <c r="B176" s="2">
         <v>42415</v>
       </c>
     </row>
@@ -5065,7 +5249,7 @@
       <c r="A178" t="s">
         <v>33</v>
       </c>
-      <c r="B178" s="6">
+      <c r="B178" s="2">
         <v>722174</v>
       </c>
     </row>
@@ -5082,7 +5266,7 @@
       <c r="A180" t="s">
         <v>33</v>
       </c>
-      <c r="B180" s="6">
+      <c r="B180" s="2">
         <v>38525</v>
       </c>
     </row>
@@ -5090,7 +5274,7 @@
       <c r="A181" t="s">
         <v>34</v>
       </c>
-      <c r="B181" s="6">
+      <c r="B181" s="2">
         <v>-38784</v>
       </c>
     </row>
@@ -5107,7 +5291,7 @@
       <c r="A183" t="s">
         <v>33</v>
       </c>
-      <c r="B183" s="6">
+      <c r="B183" s="2">
         <v>20092</v>
       </c>
     </row>
@@ -5124,7 +5308,7 @@
       <c r="A185" t="s">
         <v>33</v>
       </c>
-      <c r="B185" s="6">
+      <c r="B185" s="2">
         <v>117164</v>
       </c>
     </row>
@@ -5141,7 +5325,7 @@
       <c r="A187" t="s">
         <v>33</v>
       </c>
-      <c r="B187" s="6">
+      <c r="B187" s="2">
         <v>166726</v>
       </c>
     </row>
@@ -5158,7 +5342,7 @@
       <c r="A189" t="s">
         <v>33</v>
       </c>
-      <c r="B189" s="6">
+      <c r="B189" s="2">
         <v>61029</v>
       </c>
     </row>
@@ -5175,7 +5359,7 @@
       <c r="A191" t="s">
         <v>33</v>
       </c>
-      <c r="B191" s="6">
+      <c r="B191" s="2">
         <v>38186</v>
       </c>
     </row>
@@ -5192,7 +5376,7 @@
       <c r="A193" t="s">
         <v>33</v>
       </c>
-      <c r="B193" s="6">
+      <c r="B193" s="2">
         <v>30231</v>
       </c>
     </row>
@@ -5214,7 +5398,7 @@
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="5" t="s">
+      <c r="A196" t="s">
         <v>38</v>
       </c>
       <c r="B196" s="2">
@@ -5247,7 +5431,7 @@
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="5" t="s">
+      <c r="A200" t="s">
         <v>38</v>
       </c>
       <c r="B200" s="2">
@@ -5267,15 +5451,15 @@
       <c r="A202" t="s">
         <v>33</v>
       </c>
-      <c r="B202" s="6">
+      <c r="B202" s="2">
         <v>12542</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="5" t="s">
+      <c r="A203" t="s">
         <v>38</v>
       </c>
-      <c r="B203" s="6">
+      <c r="B203" s="2">
         <v>11365</v>
       </c>
     </row>
@@ -5292,16 +5476,16 @@
       <c r="A205" t="s">
         <v>33</v>
       </c>
-      <c r="B205" s="6">
+      <c r="B205" s="2">
         <f>25244-3623+75940</f>
         <v>97561</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="5" t="s">
+      <c r="A206" t="s">
         <v>38</v>
       </c>
-      <c r="B206" s="6">
+      <c r="B206" s="2">
         <f>1153+25788</f>
         <v>26941</v>
       </c>
@@ -5310,7 +5494,7 @@
       <c r="A207" t="s">
         <v>34</v>
       </c>
-      <c r="B207" s="6">
+      <c r="B207" s="2">
         <v>-17881</v>
       </c>
     </row>
@@ -5745,7 +5929,7 @@
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="5" t="s">
+      <c r="A266" t="s">
         <v>92</v>
       </c>
       <c r="B266" s="2">
@@ -5753,7 +5937,7 @@
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="5" t="s">
+      <c r="A267" t="s">
         <v>93</v>
       </c>
       <c r="B267" s="2">
@@ -5770,7 +5954,7 @@
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="5" t="s">
+      <c r="A269" t="s">
         <v>95</v>
       </c>
       <c r="B269" s="2">
@@ -5778,7 +5962,7 @@
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="5" t="s">
+      <c r="A270" t="s">
         <v>96</v>
       </c>
       <c r="B270" s="2">
@@ -5818,6 +6002,395 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B9B03A-61A1-40E0-9030-CF65AD818B06}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2">
+        <v>819901</v>
+      </c>
+      <c r="D1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2">
+        <f>B1+B2</f>
+        <v>810408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-9493</v>
+      </c>
+      <c r="D2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2">
+        <f>B4+B5</f>
+        <v>1364228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="4">
+        <f>B1+B2</f>
+        <v>810408</v>
+      </c>
+      <c r="D3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2">
+        <f>B7+B9</f>
+        <v>1527772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1364918</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2">
+        <f>B8</f>
+        <v>2084821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-690</v>
+      </c>
+      <c r="D5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2">
+        <f>B11+B12</f>
+        <v>684792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="4">
+        <f>SUM(B4:B5)</f>
+        <v>1364228</v>
+      </c>
+      <c r="D6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2">
+        <f>B14+B16</f>
+        <v>255728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1690205</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2">
+        <f>B15</f>
+        <v>77742</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2084821</v>
+      </c>
+      <c r="D8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="2">
+        <f>B18+B20</f>
+        <v>326899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-162433</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="2">
+        <f>B19</f>
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="4">
+        <f>SUM(B7:B9)</f>
+        <v>3612593</v>
+      </c>
+      <c r="D10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2">
+        <f>B22+B24</f>
+        <v>922615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2">
+        <v>686271</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2">
+        <f>B23</f>
+        <v>83792</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-1479</v>
+      </c>
+      <c r="D12" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="2">
+        <f>B26+B28</f>
+        <v>375578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="4">
+        <f>SUM(B11:B12)</f>
+        <v>684792</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2">
+        <f>B27</f>
+        <v>196492</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2">
+        <v>276433</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2">
+        <v>77742</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2">
+        <v>-20705</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="4">
+        <f>SUM(B14:B16)</f>
+        <v>333470</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2">
+        <v>330022</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-3123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="4">
+        <f>SUM(B18:B20)</f>
+        <v>330257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2">
+        <v>962862</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2">
+        <v>83792</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2">
+        <v>-40247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="4">
+        <f>SUM(B22:B24)</f>
+        <v>1006407</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="2">
+        <v>431203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2">
+        <v>196492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="2">
+        <v>-55625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="4">
+        <f>SUM(B26:B28)</f>
+        <v>572070</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE86B32-F4EB-4C5E-9E88-B60995AAC991}">
   <dimension ref="A3:D18"/>
   <sheetViews>

</xml_diff>